<commit_message>
Now can read Jutarnji List articles
</commit_message>
<xml_diff>
--- a/pitanje.xlsx
+++ b/pitanje.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snc/Box/Škola/HR/Croatian-sentimentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83F2D960-05FF-4E42-ABA4-3BA1DFFE18A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CD0023-6F5C-834B-AC06-FEA625504E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{80BADFDB-86D8-B241-A58A-329066326B0A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Rečenica</t>
   </si>
@@ -51,13 +51,63 @@
   </si>
   <si>
     <t>https://www.24sata.hr/news/ljubicic-on-je-iz-zagreba-ne-zna-da-more-tako-ne-izgleda-648751</t>
+  </si>
+  <si>
+    <t>Zreo da podleti pod auto ako bi se i uspio ustati</t>
+  </si>
+  <si>
+    <t>https://dnevnik.hr/vijesti/hrvatska/igor-skoko-na-facebooku-podijelio-iskustvo-s-ulice---575287.html</t>
+  </si>
+  <si>
+    <t>19-09-15-22.33</t>
+  </si>
+  <si>
+    <t>No istraga protiv Letića srpske je tužitelje navodno dovela do novih nevjerojatnih sumnji o njegovim kriminalnim radnjama.</t>
+  </si>
+  <si>
+    <t>Example of difficulty to classify</t>
+  </si>
+  <si>
+    <t>19-09-15-23.01</t>
+  </si>
+  <si>
+    <r>
+      <t>Liječnici nam se ipak vraćaju, shvaćaju da nije</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> u šoldima</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sve!'</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.24sata.hr/news/lijecnici-nam-se-ipak-vracaju-shvacaju-da-nije-u-soldima-sve-648900</t>
+  </si>
+  <si>
+    <t>19-09-16-11.19</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,6 +119,14 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,9 +153,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -413,49 +472,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1627E8BA-6DE6-3347-B49A-0CE6ED0BB2F8}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="119.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" customWidth="1"/>
-    <col min="3" max="3" width="123.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
-        <v>5</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{8D9C68EA-1DFE-8043-A810-2E618704476F}"/>
+    <hyperlink ref="C3" r:id="rId1" xr:uid="{8D9C68EA-1DFE-8043-A810-2E618704476F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Improvements to breaking up sentences from Novi List
</commit_message>
<xml_diff>
--- a/pitanje.xlsx
+++ b/pitanje.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/snc/Box/Škola/HR/Croatian-sentimentAnalysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CD0023-6F5C-834B-AC06-FEA625504E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05658F11-86F6-5648-90FA-C82D27D491D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{80BADFDB-86D8-B241-A58A-329066326B0A}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Rečenica</t>
   </si>
@@ -101,6 +101,114 @@
   </si>
   <si>
     <t>19-09-16-11.19</t>
+  </si>
+  <si>
+    <t>Europska komisija je bi sredinom sljedećeg mjeseca trebala dati pozitivnu ocjenu da je Hrvatska ispunila sve kriterije za ulazak u šengenski prostor</t>
+  </si>
+  <si>
+    <t>https://www.24sata.hr/news/bitno-je-dobiti-zeleno-svjetlo-ulazak-ne-mozemo-predvidjeto-650975</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">U tom pravcu, nama je interes da se </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>hladne glave</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pristupi svemu.</t>
+    </r>
+  </si>
+  <si>
+    <t>http://novilist.hr/Vijesti/Hrvatska/Kristianova-majka-ne-zeli-da-se-ikome-vise-ponovi-ono-sto-je-ubilo-njenog-sina-Trazimo-pravdu</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nitko</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dosad nije </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>imao</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ovako kompleksne uvjete za Schengen«, izjavio je Božinović u intervjuu za Mediaservis</t>
+    </r>
+  </si>
+  <si>
+    <t>http://novilist.hr/Vijesti/Hrvatska/PITANJE-SCHENGENA-Slovenija-brusi-alate-za-blokadu-Hrvatske?meta_refresh=true</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Župani su u subotu bili gosti Festivala voća </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>u mjestu Tavankut</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, a zatim…</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -178,7 +286,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Bureau">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -216,7 +324,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Bureau">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -322,7 +430,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Bureau">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -472,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1627E8BA-6DE6-3347-B49A-0CE6ED0BB2F8}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="157" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,12 +604,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -512,7 +620,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -523,7 +631,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -534,7 +642,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -543,6 +651,35 @@
       </c>
       <c r="C6" t="s">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>